<commit_message>
Change cooling and PV
Cooling Y all multiplied *COP=4,3
Run with new PV profiles, adjusted to meet total production kWh

Failed try changing HW storage settings
</commit_message>
<xml_diff>
--- a/tesi_camilla/casi_MarioU/results_database.xlsx
+++ b/tesi_camilla/casi_MarioU/results_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cami/Documents/GitHub/pyesm_thesis/tesi_camilla/casi_MarioU/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93820C3-AEB8-9B47-AB0B-17054C711BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6902DE-016C-1E4E-8173-686596F73BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$C$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -252,9 +265,7 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -615,7 +626,7 @@
   <dimension ref="A1:AB13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -716,23 +727,23 @@
       <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" t="s">
         <v>30</v>
       </c>
       <c r="D2">
-        <v>15604.07</v>
+        <v>23484.81</v>
       </c>
       <c r="E2">
-        <v>1214.93</v>
+        <v>1992.98</v>
       </c>
       <c r="F2">
-        <v>5500</v>
+        <v>6910</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <v>3</v>
@@ -759,69 +770,69 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R2">
-        <v>4699.63</v>
+        <v>4132.87</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>1645.58</v>
       </c>
       <c r="T2">
-        <v>4699.63</v>
+        <v>2908.77</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>404.46</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <v>1628.56</v>
       </c>
       <c r="W2">
-        <v>939.93</v>
+        <v>581.75</v>
       </c>
       <c r="X2">
-        <v>0</v>
+        <v>-18.850000000000001</v>
       </c>
       <c r="Y2">
-        <v>1214.93</v>
+        <v>837.91</v>
       </c>
       <c r="Z2">
-        <v>0</v>
+        <v>905.07</v>
       </c>
       <c r="AA2">
-        <v>0</v>
+        <v>1075.07</v>
       </c>
       <c r="AB2">
-        <v>12984.529200000001</v>
+        <v>41206.579299999998</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" t="s">
         <v>32</v>
       </c>
       <c r="D3">
-        <v>22007.4</v>
+        <v>18151.439999999999</v>
       </c>
       <c r="E3">
-        <v>1804.51</v>
+        <v>1364.91</v>
       </c>
       <c r="F3">
-        <v>7000</v>
+        <v>6800</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -851,13 +862,13 @@
         <v>4</v>
       </c>
       <c r="R3">
-        <v>3859.69</v>
+        <v>1935.67</v>
       </c>
       <c r="S3">
-        <v>950.13</v>
+        <v>941.42</v>
       </c>
       <c r="T3">
-        <v>3859.69</v>
+        <v>1935.67</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -866,39 +877,39 @@
         <v>0</v>
       </c>
       <c r="W3">
-        <v>771.94</v>
+        <v>387.13</v>
       </c>
       <c r="X3">
         <v>0</v>
       </c>
       <c r="Y3">
-        <v>1071.94</v>
+        <v>637.13</v>
       </c>
       <c r="Z3">
-        <v>522.57000000000005</v>
+        <v>517.78</v>
       </c>
       <c r="AA3">
-        <v>692.57</v>
+        <v>687.78</v>
       </c>
       <c r="AB3">
-        <v>30043.392899999999</v>
+        <v>25287.2893</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" t="s">
         <v>34</v>
       </c>
       <c r="D4">
-        <v>25993.51</v>
+        <v>26066.29</v>
       </c>
       <c r="E4">
-        <v>2025.29</v>
+        <v>2034.04</v>
       </c>
       <c r="F4">
         <v>9150</v>
@@ -937,13 +948,13 @@
         <v>4</v>
       </c>
       <c r="R4">
-        <v>3919.42</v>
+        <v>3982.3</v>
       </c>
       <c r="S4">
-        <v>1375.28</v>
+        <v>1368.32</v>
       </c>
       <c r="T4">
-        <v>3919.42</v>
+        <v>3982.3</v>
       </c>
       <c r="U4">
         <v>0</v>
@@ -952,39 +963,39 @@
         <v>0</v>
       </c>
       <c r="W4">
-        <v>783.88</v>
+        <v>796.46</v>
       </c>
       <c r="X4">
         <v>0</v>
       </c>
       <c r="Y4">
-        <v>1058.8800000000001</v>
+        <v>1071.46</v>
       </c>
       <c r="Z4">
-        <v>756.4</v>
+        <v>752.58</v>
       </c>
       <c r="AA4">
-        <v>926.4</v>
+        <v>922.58</v>
       </c>
       <c r="AB4">
-        <v>39099.0628</v>
+        <v>39110.735000000001</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" t="s">
         <v>36</v>
       </c>
       <c r="D5">
-        <v>31031.31</v>
+        <v>30650.97</v>
       </c>
       <c r="E5">
-        <v>2348.4699999999998</v>
+        <v>2302.7399999999998</v>
       </c>
       <c r="F5">
         <v>11500</v>
@@ -1023,13 +1034,13 @@
         <v>4</v>
       </c>
       <c r="R5">
-        <v>4365.05</v>
+        <v>4168.38</v>
       </c>
       <c r="S5">
-        <v>1755.39</v>
+        <v>1743.75</v>
       </c>
       <c r="T5">
-        <v>4365.05</v>
+        <v>4168.38</v>
       </c>
       <c r="U5">
         <v>0</v>
@@ -1038,45 +1049,45 @@
         <v>0</v>
       </c>
       <c r="W5">
-        <v>873.01</v>
+        <v>833.68</v>
       </c>
       <c r="X5">
         <v>0</v>
       </c>
       <c r="Y5">
-        <v>1173.01</v>
+        <v>1133.68</v>
       </c>
       <c r="Z5">
-        <v>965.46</v>
+        <v>959.06</v>
       </c>
       <c r="AA5">
-        <v>1135.46</v>
+        <v>1129.06</v>
       </c>
       <c r="AB5">
-        <v>48189.5239</v>
+        <v>47489.95</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" t="s">
         <v>30</v>
       </c>
       <c r="D6">
-        <v>17878.34</v>
+        <v>24825.84</v>
       </c>
       <c r="E6">
-        <v>1276.76</v>
+        <v>1942.6</v>
       </c>
       <c r="F6">
-        <v>7260</v>
+        <v>8670</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6">
         <v>3</v>
@@ -1103,69 +1114,69 @@
         <v>0</v>
       </c>
       <c r="P6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R6">
-        <v>6039.89</v>
+        <v>5167.28</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <v>1426.17</v>
       </c>
       <c r="T6">
-        <v>4654.8599999999997</v>
+        <v>3475.46</v>
       </c>
       <c r="U6">
-        <v>197.58</v>
+        <v>1328.06</v>
       </c>
       <c r="V6">
-        <v>1582.61</v>
+        <v>3019.87</v>
       </c>
       <c r="W6">
-        <v>930.97</v>
+        <v>695.09</v>
       </c>
       <c r="X6">
-        <v>-9.2100000000000009</v>
+        <v>-61.89</v>
       </c>
       <c r="Y6">
-        <v>1196.76</v>
+        <v>908.21</v>
       </c>
       <c r="Z6">
-        <v>0</v>
+        <v>784.4</v>
       </c>
       <c r="AA6">
-        <v>0</v>
+        <v>954.4</v>
       </c>
       <c r="AB6">
-        <v>18155.897300000001</v>
+        <v>39188.255599999997</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" t="s">
         <v>32</v>
       </c>
       <c r="D7">
-        <v>27023.4</v>
+        <v>21071.89</v>
       </c>
       <c r="E7">
-        <v>2208.04</v>
+        <v>1728.1</v>
       </c>
       <c r="F7">
-        <v>8660</v>
+        <v>6700</v>
       </c>
       <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>1</v>
-      </c>
-      <c r="H7">
-        <v>3</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1195,54 +1206,54 @@
         <v>4</v>
       </c>
       <c r="R7">
-        <v>4159.62</v>
+        <v>1677.58</v>
       </c>
       <c r="S7">
-        <v>1930.32</v>
+        <v>1741.05</v>
       </c>
       <c r="T7">
-        <v>3007.01</v>
+        <v>1677.58</v>
       </c>
       <c r="U7">
-        <v>430</v>
+        <v>0</v>
       </c>
       <c r="V7">
-        <v>1582.61</v>
+        <v>0</v>
       </c>
       <c r="W7">
-        <v>601.4</v>
+        <v>335.52</v>
       </c>
       <c r="X7">
-        <v>-20.04</v>
+        <v>0</v>
       </c>
       <c r="Y7">
-        <v>856.36</v>
+        <v>560.52</v>
       </c>
       <c r="Z7">
-        <v>1061.68</v>
+        <v>957.58</v>
       </c>
       <c r="AA7">
-        <v>1231.68</v>
+        <v>1127.58</v>
       </c>
       <c r="AB7">
-        <v>50119.927799999998</v>
+        <v>42412.075100000002</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" t="s">
         <v>34</v>
       </c>
       <c r="D8">
-        <v>33529.96</v>
+        <v>31834.38</v>
       </c>
       <c r="E8">
-        <v>2931.48</v>
+        <v>2727.6</v>
       </c>
       <c r="F8">
         <v>9150</v>
@@ -1281,13 +1292,13 @@
         <v>4</v>
       </c>
       <c r="R8">
-        <v>4241.76</v>
+        <v>4004.17</v>
       </c>
       <c r="S8">
-        <v>2905.69</v>
+        <v>2621.39</v>
       </c>
       <c r="T8">
-        <v>4241.76</v>
+        <v>4004.17</v>
       </c>
       <c r="U8">
         <v>0</v>
@@ -1296,39 +1307,39 @@
         <v>0</v>
       </c>
       <c r="W8">
-        <v>848.35</v>
+        <v>800.83</v>
       </c>
       <c r="X8">
         <v>0</v>
       </c>
       <c r="Y8">
-        <v>1123.3499999999999</v>
+        <v>1075.83</v>
       </c>
       <c r="Z8">
-        <v>1598.13</v>
+        <v>1441.77</v>
       </c>
       <c r="AA8">
-        <v>1768.13</v>
+        <v>1611.77</v>
       </c>
       <c r="AB8">
-        <v>74960.680500000002</v>
+        <v>68485.450700000001</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" t="s">
         <v>36</v>
       </c>
       <c r="D9">
-        <v>40402.519999999997</v>
+        <v>38440.17</v>
       </c>
       <c r="E9">
-        <v>3475.28</v>
+        <v>3239.32</v>
       </c>
       <c r="F9">
         <v>11500</v>
@@ -1367,13 +1378,13 @@
         <v>4</v>
       </c>
       <c r="R9">
-        <v>4322.71</v>
+        <v>4186.0600000000004</v>
       </c>
       <c r="S9">
-        <v>3819.52</v>
+        <v>3440.2</v>
       </c>
       <c r="T9">
-        <v>4322.71</v>
+        <v>4186.0600000000004</v>
       </c>
       <c r="U9">
         <v>0</v>
@@ -1382,51 +1393,51 @@
         <v>0</v>
       </c>
       <c r="W9">
-        <v>864.54</v>
+        <v>837.21</v>
       </c>
       <c r="X9">
         <v>0</v>
       </c>
       <c r="Y9">
-        <v>1164.54</v>
+        <v>1137.21</v>
       </c>
       <c r="Z9">
-        <v>2100.7399999999998</v>
+        <v>1892.11</v>
       </c>
       <c r="AA9">
-        <v>2270.7399999999998</v>
+        <v>2062.11</v>
       </c>
       <c r="AB9">
-        <v>93871.930900000007</v>
+        <v>85861.739400000006</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" t="s">
         <v>30</v>
       </c>
       <c r="D10">
-        <v>18951.43</v>
+        <v>25690.400000000001</v>
       </c>
       <c r="E10">
-        <v>1719.62</v>
+        <v>1878.22</v>
       </c>
       <c r="F10">
-        <v>4650</v>
+        <v>10070</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10">
         <v>3</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
       </c>
       <c r="J10">
         <v>24</v>
@@ -1453,63 +1464,63 @@
         <v>4</v>
       </c>
       <c r="R10">
-        <v>2864.15</v>
+        <v>2899.97</v>
       </c>
       <c r="S10">
-        <v>1203.26</v>
+        <v>2204.3000000000002</v>
       </c>
       <c r="T10">
-        <v>2864.15</v>
+        <v>827.81</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>852.11</v>
       </c>
       <c r="V10">
-        <v>0</v>
+        <v>2724.15</v>
       </c>
       <c r="W10">
-        <v>572.83000000000004</v>
+        <v>165.56</v>
       </c>
       <c r="X10">
-        <v>0</v>
+        <v>-39.71</v>
       </c>
       <c r="Y10">
-        <v>847.83</v>
+        <v>375.85</v>
       </c>
       <c r="Z10">
-        <v>661.79</v>
+        <v>1212.3599999999999</v>
       </c>
       <c r="AA10">
-        <v>831.79</v>
+        <v>1382.36</v>
       </c>
       <c r="AB10">
-        <v>36481.025600000001</v>
+        <v>47453.356800000001</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" t="s">
         <v>32</v>
       </c>
       <c r="D11">
-        <v>27993.48</v>
+        <v>23074.720000000001</v>
       </c>
       <c r="E11">
-        <v>2524.29</v>
+        <v>1968.92</v>
       </c>
       <c r="F11">
-        <v>7000</v>
+        <v>6700</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -1539,13 +1550,13 @@
         <v>4</v>
       </c>
       <c r="R11">
-        <v>3682.71</v>
+        <v>1290.45</v>
       </c>
       <c r="S11">
-        <v>2323.17</v>
+        <v>2319.69</v>
       </c>
       <c r="T11">
-        <v>3682.71</v>
+        <v>1290.45</v>
       </c>
       <c r="U11">
         <v>0</v>
@@ -1554,39 +1565,39 @@
         <v>0</v>
       </c>
       <c r="W11">
-        <v>736.54</v>
+        <v>258.08999999999997</v>
       </c>
       <c r="X11">
         <v>0</v>
       </c>
       <c r="Y11">
-        <v>1036.54</v>
+        <v>483.09</v>
       </c>
       <c r="Z11">
-        <v>1277.74</v>
+        <v>1275.83</v>
       </c>
       <c r="AA11">
-        <v>1447.74</v>
+        <v>1445.83</v>
       </c>
       <c r="AB11">
-        <v>62370.230100000001</v>
+        <v>53043.0864</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" t="s">
         <v>34</v>
       </c>
       <c r="D12">
-        <v>35846.629999999997</v>
+        <v>35765.550000000003</v>
       </c>
       <c r="E12">
-        <v>3210.04</v>
+        <v>3200.29</v>
       </c>
       <c r="F12">
         <v>9150</v>
@@ -1625,13 +1636,13 @@
         <v>4</v>
       </c>
       <c r="R12">
-        <v>3972.2</v>
+        <v>3912.73</v>
       </c>
       <c r="S12">
-        <v>3510.18</v>
+        <v>3514.08</v>
       </c>
       <c r="T12">
-        <v>3972.2</v>
+        <v>3912.73</v>
       </c>
       <c r="U12">
         <v>0</v>
@@ -1640,39 +1651,39 @@
         <v>0</v>
       </c>
       <c r="W12">
-        <v>794.44</v>
+        <v>782.55</v>
       </c>
       <c r="X12">
         <v>0</v>
       </c>
       <c r="Y12">
-        <v>1069.44</v>
+        <v>1057.55</v>
       </c>
       <c r="Z12">
-        <v>1930.6</v>
+        <v>1932.75</v>
       </c>
       <c r="AA12">
-        <v>2100.6</v>
+        <v>2102.75</v>
       </c>
       <c r="AB12">
-        <v>87534.576199999996</v>
+        <v>87381.915500000003</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" t="s">
         <v>36</v>
       </c>
       <c r="D13">
-        <v>43910.26</v>
+        <v>43584.84</v>
       </c>
       <c r="E13">
-        <v>3897.05</v>
+        <v>3857.92</v>
       </c>
       <c r="F13">
         <v>11500</v>
@@ -1711,13 +1722,13 @@
         <v>4</v>
       </c>
       <c r="R13">
-        <v>4320.09</v>
+        <v>4108.26</v>
       </c>
       <c r="S13">
-        <v>4587.34</v>
+        <v>4593.22</v>
       </c>
       <c r="T13">
-        <v>4320.09</v>
+        <v>4108.26</v>
       </c>
       <c r="U13">
         <v>0</v>
@@ -1726,22 +1737,22 @@
         <v>0</v>
       </c>
       <c r="W13">
-        <v>864.02</v>
+        <v>821.65</v>
       </c>
       <c r="X13">
         <v>0</v>
       </c>
       <c r="Y13">
-        <v>1164.02</v>
+        <v>1121.6500000000001</v>
       </c>
       <c r="Z13">
-        <v>2523.04</v>
+        <v>2526.27</v>
       </c>
       <c r="AA13">
-        <v>2693.04</v>
+        <v>2696.27</v>
       </c>
       <c r="AB13">
-        <v>110753.2798</v>
+        <v>110050.3893</v>
       </c>
     </row>
   </sheetData>

</xml_diff>